<commit_message>
Update in the simulation
</commit_message>
<xml_diff>
--- a/Final Analysis.xlsx
+++ b/Final Analysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="460" windowWidth="33600" windowHeight="19760" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,57 +36,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t>[]</t>
-  </si>
-  <si>
-    <t>[100,100,1000,0.0015]</t>
-  </si>
-  <si>
-    <t>[100,200,1000,0.0015]</t>
-  </si>
-  <si>
-    <t>[100,300,1000,0.0015]</t>
-  </si>
-  <si>
-    <t>[100,400,1000,0.0015]</t>
-  </si>
-  <si>
-    <t>[200,100,1000,0.0015]</t>
-  </si>
-  <si>
-    <t>[200,200,1000,0.0015]</t>
-  </si>
-  <si>
-    <t>[200,300,1000,0.0015]</t>
-  </si>
-  <si>
-    <t>[200,400,1000,0.0015]</t>
-  </si>
-  <si>
-    <t>[300,100,1000,0.0015]</t>
-  </si>
-  <si>
-    <t>[300,200,1000,0.0015]</t>
-  </si>
-  <si>
-    <t>[300,300,1000,0.0015]</t>
-  </si>
-  <si>
-    <t>[300,400,1000,0.0015]</t>
-  </si>
-  <si>
-    <t>[400,100,1000,0.0015]</t>
-  </si>
-  <si>
-    <t>[400,200,1000,0.0015]</t>
-  </si>
-  <si>
-    <t>[400,300,1000,0.0015]</t>
-  </si>
-  <si>
-    <t>[400,400,1000,0.0015]</t>
   </si>
   <si>
     <t>TotalTime</t>
@@ -159,6 +111,12 @@
   </si>
   <si>
     <t>BlockTime</t>
+  </si>
+  <si>
+    <t>[100,100,95000,0.0015]</t>
+  </si>
+  <si>
+    <t>[200,200,95000,0.0015]</t>
   </si>
 </sst>
 </file>
@@ -276,7 +234,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$B$20</c:f>
+              <c:f>Sheet1!$B$2:$B$6</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -299,7 +257,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$20</c:f>
+              <c:f>Sheet1!$C$2:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -336,8 +294,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1066949456"/>
-        <c:axId val="-1066947680"/>
+        <c:axId val="-969288112"/>
+        <c:axId val="-969285792"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -362,7 +320,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$B$20</c:f>
+              <c:f>Sheet1!$B$2:$B$6</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -385,7 +343,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$20</c:f>
+              <c:f>Sheet1!$F$2:$F$6</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="5"/>
@@ -424,11 +382,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1066942080"/>
-        <c:axId val="-1066944624"/>
+        <c:axId val="-969278496"/>
+        <c:axId val="-969281888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1066949456"/>
+        <c:axId val="-969288112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -471,7 +429,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1066947680"/>
+        <c:crossAx val="-969285792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -479,7 +437,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1066947680"/>
+        <c:axId val="-969285792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -598,12 +556,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1066949456"/>
+        <c:crossAx val="-969288112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1066944624"/>
+        <c:axId val="-969281888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -700,12 +658,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1066942080"/>
+        <c:crossAx val="-969278496"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-1066942080"/>
+        <c:axId val="-969278496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -729,7 +687,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1066944624"/>
+        <c:crossAx val="-969281888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -874,7 +832,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$B$20</c:f>
+              <c:f>Sheet1!$B$2:$B$6</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -897,7 +855,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$20</c:f>
+              <c:f>Sheet1!$F$2:$F$6</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="5"/>
@@ -930,11 +888,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1066520608"/>
-        <c:axId val="-1066518288"/>
+        <c:axId val="-969257040"/>
+        <c:axId val="-969254720"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1066520608"/>
+        <c:axId val="-969257040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -977,7 +935,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1066518288"/>
+        <c:crossAx val="-969254720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -985,7 +943,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1066518288"/>
+        <c:axId val="-969254720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1932.0"/>
@@ -1037,7 +995,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1066520608"/>
+        <c:crossAx val="-969257040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1204,7 +1162,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$B$20</c:f>
+              <c:f>Sheet1!$B$2:$B$6</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1227,7 +1185,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$20</c:f>
+              <c:f>Sheet1!$C$2:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1278,7 +1236,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$B$20</c:f>
+              <c:f>Sheet1!$B$2:$B$6</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1301,7 +1259,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$20</c:f>
+              <c:f>Sheet1!$D$2:$D$6</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1334,11 +1292,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1066325712"/>
-        <c:axId val="-1066323392"/>
+        <c:axId val="-968970816"/>
+        <c:axId val="-968969040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1066325712"/>
+        <c:axId val="-968970816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1381,7 +1339,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1066323392"/>
+        <c:crossAx val="-968969040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1389,7 +1347,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1066323392"/>
+        <c:axId val="-968969040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1439,7 +1397,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1066325712"/>
+        <c:crossAx val="-968970816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1664,8 +1622,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1014914496"/>
-        <c:axId val="-692658672"/>
+        <c:axId val="-969016560"/>
+        <c:axId val="-969014512"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1752,11 +1710,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-694476192"/>
-        <c:axId val="-692654768"/>
+        <c:axId val="-969790320"/>
+        <c:axId val="-798029824"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1014914496"/>
+        <c:axId val="-969016560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1799,7 +1757,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-692658672"/>
+        <c:crossAx val="-969014512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1807,7 +1765,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-692658672"/>
+        <c:axId val="-969014512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1926,12 +1884,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1014914496"/>
+        <c:crossAx val="-969016560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-692654768"/>
+        <c:axId val="-798029824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2028,12 +1986,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-694476192"/>
+        <c:crossAx val="-969790320"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-694476192"/>
+        <c:axId val="-969790320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2057,7 +2015,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-692654768"/>
+        <c:crossAx val="-798029824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2258,11 +2216,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-694563200"/>
-        <c:axId val="-694560880"/>
+        <c:axId val="-969079216"/>
+        <c:axId val="-969058704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-694563200"/>
+        <c:axId val="-969079216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2305,7 +2263,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-694560880"/>
+        <c:crossAx val="-969058704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2313,7 +2271,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-694560880"/>
+        <c:axId val="-969058704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1932.0"/>
@@ -2365,7 +2323,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-694563200"/>
+        <c:crossAx val="-969079216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2662,11 +2620,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-694820016"/>
-        <c:axId val="-992717040"/>
+        <c:axId val="-969737696"/>
+        <c:axId val="-969735376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-694820016"/>
+        <c:axId val="-969737696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2709,7 +2667,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-992717040"/>
+        <c:crossAx val="-969735376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2717,7 +2675,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-992717040"/>
+        <c:axId val="-969735376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2767,7 +2725,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-694820016"/>
+        <c:crossAx val="-969737696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6180,7 +6138,7 @@
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>380599</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>86500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6188,7 +6146,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32A7E352-9AFD-438E-8D30-943810E5B8A4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{32A7E352-9AFD-438E-8D30-943810E5B8A4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6218,7 +6176,7 @@
     <xdr:to>
       <xdr:col>35</xdr:col>
       <xdr:colOff>647300</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>137300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6242,13 +6200,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>184150</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>158750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>386950</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>118250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6291,7 +6249,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32A7E352-9AFD-438E-8D30-943810E5B8A4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{32A7E352-9AFD-438E-8D30-943810E5B8A4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6379,8 +6337,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H20" totalsRowShown="0">
-  <autoFilter ref="A1:H20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H6" totalsRowShown="0">
+  <autoFilter ref="A1:H6"/>
   <tableColumns count="8">
     <tableColumn id="1" name="TotalTime"/>
     <tableColumn id="2" name="Alg"/>
@@ -6708,10 +6666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6720,35 +6678,35 @@
     <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="H1" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -6756,7 +6714,7 @@
         <v>80.634422540664602</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1">
         <v>3.2661457061767501E-3</v>
@@ -6782,7 +6740,7 @@
         <v>88.773266077041598</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1">
         <v>1.01193258762359E-2</v>
@@ -6808,7 +6766,7 @@
         <v>261.28573536872801</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1">
         <v>0.107951204061508</v>
@@ -6834,7 +6792,7 @@
         <v>175.782389879226</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1">
         <v>4.5596263408660798E-2</v>
@@ -6843,7 +6801,7 @@
         <v>0.170412564992904</v>
       </c>
       <c r="E5" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="F5" s="2">
         <v>1931.80959999997</v>
@@ -6855,394 +6813,30 @@
         <v>999864</v>
       </c>
     </row>
-    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>179.39047718047999</v>
-      </c>
-      <c r="B6">
-        <v>3</v>
+        <v>221.80209994316101</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
       </c>
       <c r="C6" s="1">
-        <v>4.5716323852539001E-2</v>
+        <v>8.2329480648040701E-2</v>
       </c>
       <c r="D6" s="1">
-        <v>0.17127607202529899</v>
+        <v>0.20872335052490201</v>
       </c>
       <c r="E6" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="F6" s="2">
-        <v>1931.9053999999701</v>
+        <v>1932.01809999997</v>
       </c>
       <c r="G6">
-        <v>2991</v>
+        <v>2946</v>
       </c>
       <c r="H6">
-        <v>999906</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>182.93207669258101</v>
-      </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="C7" s="1">
-        <v>4.6665263891219999E-2</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0.17267457962036101</v>
-      </c>
-      <c r="E7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" s="2">
-        <v>1931.8660999999699</v>
-      </c>
-      <c r="G7">
-        <v>2991</v>
-      </c>
-      <c r="H7">
-        <v>999878</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>186.073899984359</v>
-      </c>
-      <c r="B8">
-        <v>3</v>
-      </c>
-      <c r="C8" s="1">
-        <v>4.6263180971145602E-2</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0.17319917559623699</v>
-      </c>
-      <c r="E8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" s="2">
-        <v>1931.9053999999701</v>
-      </c>
-      <c r="G8">
-        <v>2991</v>
-      </c>
-      <c r="H8">
-        <v>999906</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>215.94081735610899</v>
-      </c>
-      <c r="B9">
-        <v>3</v>
-      </c>
-      <c r="C9" s="1">
-        <v>8.18922793865203E-2</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0.20774093961715601</v>
-      </c>
-      <c r="E9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" s="2">
-        <v>1931.94279999997</v>
-      </c>
-      <c r="G9">
-        <v>2948</v>
-      </c>
-      <c r="H9">
-        <v>999819</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>221.80209994316101</v>
-      </c>
-      <c r="B10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="1">
-        <v>8.2329480648040701E-2</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0.20872335052490201</v>
-      </c>
-      <c r="E10" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10" s="2">
-        <v>1932.01809999997</v>
-      </c>
-      <c r="G10">
-        <v>2946</v>
-      </c>
-      <c r="H10">
         <v>999870</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>228.61768245696999</v>
-      </c>
-      <c r="B11">
-        <v>3</v>
-      </c>
-      <c r="C11">
-        <v>8.2780257463455201E-2</v>
-      </c>
-      <c r="D11">
-        <v>0.210109134674072</v>
-      </c>
-      <c r="E11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11">
-        <v>1932.1962999999701</v>
-      </c>
-      <c r="G11">
-        <v>2949</v>
-      </c>
-      <c r="H11">
-        <v>999997</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>237.045621395111</v>
-      </c>
-      <c r="B12">
-        <v>3</v>
-      </c>
-      <c r="C12">
-        <v>8.3630171537399295E-2</v>
-      </c>
-      <c r="D12">
-        <v>0.21234226226806599</v>
-      </c>
-      <c r="E12" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12">
-        <v>1932.12129999997</v>
-      </c>
-      <c r="G12">
-        <v>2948</v>
-      </c>
-      <c r="H12">
-        <v>999941</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>255.94495749473501</v>
-      </c>
-      <c r="B13">
-        <v>3</v>
-      </c>
-      <c r="C13">
-        <v>0.11862893295288</v>
-      </c>
-      <c r="D13">
-        <v>0.245245150804519</v>
-      </c>
-      <c r="E13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13">
-        <v>1932.07519999997</v>
-      </c>
-      <c r="G13">
-        <v>2946</v>
-      </c>
-      <c r="H13">
-        <v>999912</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>265.26621270179697</v>
-      </c>
-      <c r="B14">
-        <v>3</v>
-      </c>
-      <c r="C14">
-        <v>0.11978798270225501</v>
-      </c>
-      <c r="D14">
-        <v>0.247126488924026</v>
-      </c>
-      <c r="E14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14">
-        <v>1932.11859999997</v>
-      </c>
-      <c r="G14">
-        <v>2948</v>
-      </c>
-      <c r="H14">
-        <v>999940</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>278.19912505149802</v>
-      </c>
-      <c r="B15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15">
-        <v>0.121513720750808</v>
-      </c>
-      <c r="D15">
-        <v>0.25001849031448298</v>
-      </c>
-      <c r="E15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15">
-        <v>1932.0720999999701</v>
-      </c>
-      <c r="G15">
-        <v>2948</v>
-      </c>
-      <c r="H15">
-        <v>999907</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>289.32116985320999</v>
-      </c>
-      <c r="B16">
-        <v>3</v>
-      </c>
-      <c r="C16">
-        <v>0.121545214176177</v>
-      </c>
-      <c r="D16">
-        <v>0.25293293929100003</v>
-      </c>
-      <c r="E16" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16">
-        <v>1932.12129999997</v>
-      </c>
-      <c r="G16">
-        <v>2948</v>
-      </c>
-      <c r="H16">
-        <v>999941</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>298.597761631011</v>
-      </c>
-      <c r="B17">
-        <v>3</v>
-      </c>
-      <c r="C17">
-        <v>0.15920810985565101</v>
-      </c>
-      <c r="D17">
-        <v>0.28511043882369902</v>
-      </c>
-      <c r="E17" t="s">
-        <v>13</v>
-      </c>
-      <c r="F17">
-        <v>1931.98109999997</v>
-      </c>
-      <c r="G17">
-        <v>2944</v>
-      </c>
-      <c r="H17">
-        <v>999846</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>313.01746582984902</v>
-      </c>
-      <c r="B18">
-        <v>3</v>
-      </c>
-      <c r="C18">
-        <v>0.16021848940849301</v>
-      </c>
-      <c r="D18">
-        <v>0.288814164638519</v>
-      </c>
-      <c r="E18" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18">
-        <v>1932.16029999997</v>
-      </c>
-      <c r="G18">
-        <v>2945</v>
-      </c>
-      <c r="H18">
-        <v>999970</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>327.85086131095801</v>
-      </c>
-      <c r="B19">
-        <v>3</v>
-      </c>
-      <c r="C19">
-        <v>0.159588366031646</v>
-      </c>
-      <c r="D19">
-        <v>0.29114444231987002</v>
-      </c>
-      <c r="E19" t="s">
-        <v>15</v>
-      </c>
-      <c r="F19">
-        <v>1932.0700999999699</v>
-      </c>
-      <c r="G19">
-        <v>2948</v>
-      </c>
-      <c r="H19">
-        <v>999905</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>344.074171543121</v>
-      </c>
-      <c r="B20" t="s">
-        <v>31</v>
-      </c>
-      <c r="C20">
-        <v>0.160044483661651</v>
-      </c>
-      <c r="D20">
-        <v>0.28571750593185402</v>
-      </c>
-      <c r="E20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F20">
-        <v>1932.12129999997</v>
-      </c>
-      <c r="G20">
-        <v>2948</v>
-      </c>
-      <c r="H20">
-        <v>999941</v>
       </c>
     </row>
   </sheetData>
@@ -7258,7 +6852,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="AN2" sqref="AN2"/>
     </sheetView>
   </sheetViews>
@@ -7274,25 +6868,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="E1" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="F1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -7300,7 +6894,7 @@
         <v>80.634422540664602</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="C2">
         <v>1.0673701763153001</v>
@@ -7323,7 +6917,7 @@
         <v>88.773266077041598</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>1.1017549037933301</v>
@@ -7346,7 +6940,7 @@
         <v>261.28573536872801</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="C4">
         <v>3.3137428760528498</v>
@@ -7369,7 +6963,7 @@
         <v>175.782389879226</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="C5">
         <v>2.1976189613342201</v>
@@ -7392,7 +6986,7 @@
         <v>179.39047718047999</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="C6">
         <v>2.2563419342040998</v>
@@ -7415,7 +7009,7 @@
         <v>182.93207669258101</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="C7">
         <v>2.3137950897216699</v>
@@ -7438,7 +7032,7 @@
         <v>186.073899984359</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="C8">
         <v>2.3851830959320002</v>
@@ -7461,7 +7055,7 @@
         <v>215.94081735610899</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="C9">
         <v>2.5862069129943799</v>
@@ -7484,7 +7078,7 @@
         <v>221.80209994316101</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="C10">
         <v>2.72614192962646</v>
@@ -7599,7 +7193,7 @@
         <v>278.19912505149802</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="C15">
         <v>0.121513720750808</v>
@@ -7714,7 +7308,7 @@
         <v>344.074171543121</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="C20">
         <v>0.160044483661651</v>

</xml_diff>

<commit_message>
Final improvements on Final ALg
</commit_message>
<xml_diff>
--- a/Final Analysis.xlsx
+++ b/Final Analysis.xlsx
@@ -14,6 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
   <si>
     <t>[]</t>
   </si>
@@ -118,6 +119,21 @@
   <si>
     <t>[200,200,95000,0.0015]</t>
   </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>sdt</t>
+  </si>
+  <si>
+    <t>Knapsack</t>
+  </si>
 </sst>
 </file>
 
@@ -126,13 +142,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
     </font>
   </fonts>
   <fills count="2">
@@ -164,16 +185,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -262,19 +288,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.00326614570617675</c:v>
+                  <c:v>0.00331396055221557</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0101193258762359</c:v>
+                  <c:v>0.0101808664798736</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.107951204061508</c:v>
+                  <c:v>0.104981319189071</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0455962634086608</c:v>
+                  <c:v>0.0518476102352142</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0823294806480407</c:v>
+                  <c:v>0.0817750346660614</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1190,19 +1216,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.00326614570617675</c:v>
+                  <c:v>0.00331396055221557</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0101193258762359</c:v>
+                  <c:v>0.0101808664798736</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.107951204061508</c:v>
+                  <c:v>0.104981319189071</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0455962634086608</c:v>
+                  <c:v>0.0518476102352142</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0823294806480407</c:v>
+                  <c:v>0.0817750346660614</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1264,19 +1290,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.0786135964393615</c:v>
+                  <c:v>0.0814430658817291</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0863381164073944</c:v>
+                  <c:v>0.0896610734462738</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.257992436170578</c:v>
+                  <c:v>0.262567388772964</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.170412564992904</c:v>
+                  <c:v>0.200529457092285</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.208723350524902</c:v>
+                  <c:v>0.236512170791625</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6342,8 +6368,10 @@
   <tableColumns count="8">
     <tableColumn id="1" name="TotalTime"/>
     <tableColumn id="2" name="Alg"/>
-    <tableColumn id="3" name="Block Time"/>
-    <tableColumn id="4" name="Complete Time"/>
+    <tableColumn id="3" name="Block Time" dataDxfId="0"/>
+    <tableColumn id="4" name="Complete Time">
+      <calculatedColumnFormula>Table1[[#This Row],[TotalTime]]/1000</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="5" name="Param"/>
     <tableColumn id="6" name="Profit"/>
     <tableColumn id="7" name="# transactions"/>
@@ -6666,10 +6694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6711,16 +6739,17 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>80.634422540664602</v>
+        <v>81.443065881729098</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="1">
-        <v>3.2661457061767501E-3</v>
+        <v>3.3139605522155701E-3</v>
       </c>
       <c r="D2" s="1">
-        <v>7.8613596439361499E-2</v>
+        <f>Table1[[#This Row],[TotalTime]]/1000</f>
+        <v>8.1443065881729101E-2</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
@@ -6737,16 +6766,17 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>88.773266077041598</v>
+        <v>89.661073446273804</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="1">
-        <v>1.01193258762359E-2</v>
+        <v>1.0180866479873599E-2</v>
       </c>
       <c r="D3" s="1">
-        <v>8.6338116407394402E-2</v>
+        <f>Table1[[#This Row],[TotalTime]]/1000</f>
+        <v>8.9661073446273803E-2</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>
@@ -6763,16 +6793,17 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>261.28573536872801</v>
+        <v>262.56738877296402</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="1">
-        <v>0.107951204061508</v>
+        <v>0.104981319189071</v>
       </c>
       <c r="D4" s="1">
-        <v>0.25799243617057799</v>
+        <f>Table1[[#This Row],[TotalTime]]/1000</f>
+        <v>0.26256738877296404</v>
       </c>
       <c r="E4" t="s">
         <v>0</v>
@@ -6789,16 +6820,17 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>175.782389879226</v>
+        <v>200.52945709228501</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="1">
-        <v>4.5596263408660798E-2</v>
+        <v>5.1847610235214198E-2</v>
       </c>
       <c r="D5" s="1">
-        <v>0.170412564992904</v>
+        <f>Table1[[#This Row],[TotalTime]]/1000</f>
+        <v>0.20052945709228501</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
@@ -6815,16 +6847,17 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>221.80209994316101</v>
+        <v>236.51217079162501</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="1">
-        <v>8.2329480648040701E-2</v>
+        <v>8.1775034666061397E-2</v>
       </c>
       <c r="D6" s="1">
-        <v>0.20872335052490201</v>
+        <f>Table1[[#This Row],[TotalTime]]/1000</f>
+        <v>0.23651217079162501</v>
       </c>
       <c r="E6" t="s">
         <v>26</v>
@@ -6837,6 +6870,35 @@
       </c>
       <c r="H6">
         <v>999870</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>30</v>
+      </c>
+      <c r="B40" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>1413350.26889999</v>
+      </c>
+      <c r="B41">
+        <v>1438997.04919999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>155718.92349999899</v>
+      </c>
+      <c r="B42">
+        <v>155808.852499998</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B43">
+        <v>242926.63789999799</v>
       </c>
     </row>
   </sheetData>
@@ -6852,8 +6914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="AN2" sqref="AN2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7333,4 +7395,182 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1">
+        <v>81.443065881729098</v>
+      </c>
+      <c r="E1">
+        <v>0</v>
+      </c>
+      <c r="F1">
+        <v>3.3139605522155701E-3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1">
+        <v>1340.45849999999</v>
+      </c>
+      <c r="I1">
+        <v>2457</v>
+      </c>
+      <c r="J1">
+        <v>999925</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2">
+        <v>89.661073446273804</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1.0180866479873599E-2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>1921.49999999998</v>
+      </c>
+      <c r="I2">
+        <v>2886</v>
+      </c>
+      <c r="J2">
+        <v>999874</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3">
+        <v>262.56738877296402</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>0.104981319189071</v>
+      </c>
+      <c r="G3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>1930.86489999997</v>
+      </c>
+      <c r="I3">
+        <v>2944</v>
+      </c>
+      <c r="J3">
+        <v>999041</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4">
+        <v>200.52945709228501</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>5.1847610235214198E-2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4">
+        <v>1931.97649999997</v>
+      </c>
+      <c r="I4">
+        <v>2990</v>
+      </c>
+      <c r="J4">
+        <v>999983</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5">
+        <v>236.51217079162501</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>8.1775034666061397E-2</v>
+      </c>
+      <c r="G5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5">
+        <v>1932.01439999998</v>
+      </c>
+      <c r="I5">
+        <v>2992</v>
+      </c>
+      <c r="J5">
+        <v>999987</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>